<commit_message>
Working through first alt
</commit_message>
<xml_diff>
--- a/CH-099 Random Selection Part 2.xlsx
+++ b/CH-099 Random Selection Part 2.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACB55E2-B4B4-46DD-A15F-5D64C398E517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C15485A-58A0-4FFF-8B06-3AECBC7BEF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$3:$C$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$3:$C$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
   <si>
     <t>Question</t>
   </si>
@@ -466,8 +490,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -482,8 +506,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2482850" y="1526682"/>
-          <a:ext cx="3848100" cy="2635743"/>
+          <a:off x="2480945" y="1421907"/>
+          <a:ext cx="3823335" cy="2593833"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -869,12 +893,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1F7874B3-0D01-40BA-A740-45FD75289749}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1250,4 +1301,437 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E95D144-679E-4ADF-9EE7-BBAF65FA8994}">
+  <dimension ref="A1:L40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.8984375" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.3984375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="E1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8"/>
+      <c r="F8" s="4"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9"/>
+      <c r="F9" s="4"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10"/>
+      <c r="F10" s="4"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11"/>
+      <c r="F11" s="4"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12"/>
+      <c r="F12" s="4"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="B23:C27" ca="1">_xlfn.LET(
+    _xlpm.A, INDEX(B3:B20, _xlfn.RANDARRAY(4, 1, 1, COUNTA(B3:B20), 1), 1),
+    _xlpm.B, _xlfn.MAP(
+        _xlpm.A,
+        _xlfn.LAMBDA(_xlpm.x,
+            _xlfn.LET(
+                _xlpm.a, _xlfn._xlws.FILTER(C3:C20, B3:B20 = _xlpm.x),
+                _xlfn.CHOOSEROWS(_xlpm.a, RANDBETWEEN(1, COUNTA(_xlpm.a)))
+            )
+        )
+    ),
+    _xlfn.VSTACK({"Dep.","Staff ID"}, _xlfn.HSTACK(_xlpm.A, _xlpm.B))
+)</f>
+        <v>Dep.</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f ca="1"/>
+        <v>Staff ID</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="str">
+        <f ca="1"/>
+        <v>Production</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f ca="1"/>
+        <v>S_17</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="str">
+        <f ca="1"/>
+        <v>R&amp;D</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f ca="1"/>
+        <v>S_06</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="str">
+        <f ca="1"/>
+        <v>R&amp;D</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f ca="1"/>
+        <v>S_14</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="str">
+        <f ca="1"/>
+        <v>Production</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f ca="1"/>
+        <v>S_05</v>
+      </c>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to add a header
</commit_message>
<xml_diff>
--- a/CH-099 Random Selection Part 2.xlsx
+++ b/CH-099 Random Selection Part 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569E59AC-8467-4663-9360-47CA7F96C146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E91CD6-FE92-48AE-BF92-CE14C62DA0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1658,11 +1658,11 @@
       <c r="D23" s="1"/>
       <c r="E23" cm="1">
         <f t="array" aca="1" ref="E23:E26" ca="1">_xlfn.RANDARRAY(4,1,1,COUNTA(B3:B20),TRUE)</f>
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="F23:F26" ca="1">INDEX(B3:B20,_xlfn.ANCHORARRAY(E23))</f>
-        <v>R&amp;D</v>
+        <v>HR</v>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">_xlfn.LAMBDA(_xlpm.x,
@@ -1670,26 +1670,26 @@
 _xlpm.y, _xlfn._xlws.FILTER($C$3:$C$20,$B$3:$B$20=_xlpm.x),
 _xlpm.z, INDEX(_xlpm.y,RANDBETWEEN(1,COUNTA(_xlpm.y))),
 _xlpm.z))(F23)</f>
-        <v>S_06</v>
+        <v>S_01</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="str">
         <f ca="1"/>
-        <v>IT</v>
+        <v>R&amp;D</v>
       </c>
       <c r="C24" s="4" t="str">
         <f ca="1"/>
-        <v>S_07</v>
+        <v>S_13</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24">
         <f ca="1"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F24" t="str">
         <f ca="1"/>
-        <v>R&amp;D</v>
+        <v>IT</v>
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">_xlfn.LAMBDA(_xlpm.x,
@@ -1697,26 +1697,26 @@
 _xlpm.y, _xlfn._xlws.FILTER($C$3:$C$20,$B$3:$B$20=_xlpm.x),
 _xlpm.z, INDEX(_xlpm.y,RANDBETWEEN(1,COUNTA(_xlpm.y))),
 _xlpm.z))(F24)</f>
-        <v>S_14</v>
+        <v>S_12</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="str">
         <f ca="1"/>
-        <v>HR</v>
+        <v>IT</v>
       </c>
       <c r="C25" s="4" t="str">
         <f ca="1"/>
-        <v>S_01</v>
+        <v>S_09</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25">
         <f ca="1"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F25" t="str">
         <f ca="1"/>
-        <v>IT</v>
+        <v>Production</v>
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">_xlfn.LAMBDA(_xlpm.x,
@@ -1724,25 +1724,25 @@
 _xlpm.y, _xlfn._xlws.FILTER($C$3:$C$20,$B$3:$B$20=_xlpm.x),
 _xlpm.z, INDEX(_xlpm.y,RANDBETWEEN(1,COUNTA(_xlpm.y))),
 _xlpm.z))(F25)</f>
-        <v>S_08</v>
+        <v>S_18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="str">
         <f ca="1"/>
-        <v>Marketing</v>
+        <v>IT</v>
       </c>
       <c r="C26" s="4" t="str">
         <f ca="1"/>
-        <v>S_03</v>
+        <v>S_08</v>
       </c>
       <c r="E26">
         <f ca="1"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F26" t="str">
         <f ca="1"/>
-        <v>HR</v>
+        <v>IT</v>
       </c>
       <c r="G26" t="str" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">_xlfn.LAMBDA(_xlpm.x,
@@ -1750,17 +1750,17 @@
 _xlpm.y, _xlfn._xlws.FILTER($C$3:$C$20,$B$3:$B$20=_xlpm.x),
 _xlpm.z, INDEX(_xlpm.y,RANDBETWEEN(1,COUNTA(_xlpm.y))),
 _xlpm.z))(F26)</f>
-        <v>S_01</v>
+        <v>S_11</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="str">
         <f ca="1"/>
-        <v>R&amp;D</v>
+        <v>Marketing</v>
       </c>
       <c r="C27" s="4" t="str">
         <f ca="1"/>
-        <v>S_14</v>
+        <v>S_02</v>
       </c>
       <c r="E27"/>
     </row>
@@ -1817,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F83AA0-7245-4F01-9269-4498A7C45940}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2132,60 +2132,68 @@
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="B24:C27" ca="1">_xlfn.LET(
+      <c r="B24" s="12" t="str" cm="1">
+        <f t="array" aca="1" ref="B24:C28" ca="1">_xlfn.LET(
 _xlpm.n, INDEX(B3:B20,_xlfn.RANDARRAY(4,1,1,COUNTA(B3:B20))),
 _xlpm.fx, _xlfn.LAMBDA(_xlpm.x,
 _xlfn.LET(
 _xlpm.y, _xlfn._xlws.FILTER($C$3:$C$20,$B$3:$B$20=_xlpm.x),
 _xlpm.z, INDEX(_xlpm.y,RANDBETWEEN(1,COUNTA(_xlpm.y))),
 _xlpm.z)),
-_xlfn.HSTACK(_xlpm.n,_xlfn.MAP(_xlpm.n,_xlfn.LAMBDA(_xlpm.y,_xlpm.fx(_xlpm.y))))
+_xlfn.VSTACK(B2:C2,_xlfn.HSTACK(_xlpm.n,_xlfn.MAP(_xlpm.n,_xlfn.LAMBDA(_xlpm.y,_xlpm.fx(_xlpm.y)))))
 )</f>
-        <v>IT</v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <f ca="1"/>
-        <v>S_08</v>
+        <v>Department</v>
+      </c>
+      <c r="C24" s="10" t="str">
+        <f ca="1"/>
+        <v>Staff ID</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="str">
-        <f ca="1"/>
-        <v>R&amp;D</v>
-      </c>
-      <c r="C25" s="4" t="str">
-        <f ca="1"/>
-        <v>S_14</v>
+      <c r="B25" s="6" t="str">
+        <f ca="1"/>
+        <v>IT</v>
+      </c>
+      <c r="C25" s="11" t="str">
+        <f ca="1"/>
+        <v>S_07</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="str">
+      <c r="B26" s="6" t="str">
+        <f ca="1"/>
+        <v>Production</v>
+      </c>
+      <c r="C26" s="11" t="str">
+        <f ca="1"/>
+        <v>S_16</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="str">
         <f ca="1"/>
         <v>IT</v>
       </c>
-      <c r="C26" s="4" t="str">
-        <f ca="1"/>
-        <v>S_09</v>
-      </c>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="str">
+      <c r="C27" s="11" t="str">
+        <f ca="1"/>
+        <v>S_12</v>
+      </c>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="str">
         <f ca="1"/>
         <v>IT</v>
       </c>
-      <c r="C27" s="4" t="str">
-        <f ca="1"/>
-        <v>S_07</v>
-      </c>
-      <c r="E27"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="str">
+        <f ca="1"/>
+        <v>S_04</v>
+      </c>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>